<commit_message>
fix import by excel, master data
</commit_message>
<xml_diff>
--- a/public/EmployeeData/template-employee (1).xlsx
+++ b/public/EmployeeData/template-employee (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF93D060-C3F3-294D-A888-EF5EA52380A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42883C02-2A09-4748-9368-41696CB23152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,17 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -59,22 +53,7 @@
     <t>Department</t>
   </si>
   <si>
-    <t>Designation</t>
-  </si>
-  <si>
-    <t>Salary</t>
-  </si>
-  <si>
-    <t>Payslip Type</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Rahmat</t>
+    <t>Hidayat</t>
   </si>
   <si>
     <t>089912313213</t>
@@ -83,43 +62,46 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Ekanuri</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>Staff</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Ahmad</t>
-  </si>
-  <si>
     <t>Juantoro</t>
   </si>
   <si>
     <t>08212232133</t>
   </si>
   <si>
-    <t>Peip</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>rj@gmail.com</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>Hidayattt</t>
-  </si>
-  <si>
-    <t>aht@gmail.com</t>
+    <t>aht5@gmail.com</t>
+  </si>
+  <si>
+    <t>rj4@gmail.com</t>
+  </si>
+  <si>
+    <t>Rahmattt</t>
+  </si>
+  <si>
+    <t>Ahmaddd</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Jl. Arco Raya</t>
+  </si>
+  <si>
+    <t>Parung Panjang</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Sub Department</t>
   </si>
 </sst>
 </file>
@@ -631,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="139" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -646,99 +628,88 @@
     <col min="5" max="5" width="23.83203125" customWidth="1"/>
     <col min="7" max="7" width="14.1640625" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="10" width="13" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
+      <c r="J1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>1112</v>
+        <v>1122</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="11">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="3">
-        <v>5000000</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="I2" s="4">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3">
+        <v>33</v>
+      </c>
+      <c r="K2" s="8">
+        <v>150</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="3">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -746,43 +717,37 @@
         <v>2222</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="3">
-        <v>7400000</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="3">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="H3" s="4">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4">
+        <v>34</v>
+      </c>
+      <c r="J3" s="3">
+        <v>34</v>
+      </c>
+      <c r="K3" s="8">
+        <v>152</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -795,10 +760,8 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -811,10 +774,8 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -827,10 +788,8 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -843,10 +802,8 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -859,10 +816,8 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -875,8 +830,6 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>